<commit_message>
made changes the file
</commit_message>
<xml_diff>
--- a/CostOpt/Book1(xlsx).xlsx
+++ b/CostOpt/Book1(xlsx).xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2083475\Documents\J&amp;J\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Azure\CostOpt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
   <si>
     <t xml:space="preserve">Resource Type </t>
   </si>
@@ -534,23 +534,28 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>GET https://management.azure.com/subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/providers/Microsoft.Compute/snapshots/{snapshotName}?api-version=2023-01-01</t>
+  </si>
+  <si>
+    <t>GET https://management.azure.com/subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/providers/Microsoft.Web/sites?api-version=2023-01-01</t>
+  </si>
+  <si>
+    <t>GET https://management.azure.com/subscriptions/{subscriptionId}/resourceGroups/{resourceGroupName}/providers/Microsoft.Compute/virtualMachines/{vmName}/instanceView?api-version=2023-01-01</t>
+  </si>
+  <si>
+    <t>Refer to the Azure API documentation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="6">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,7 +631,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -634,11 +639,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -648,26 +653,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -953,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1130,7 +1135,9 @@
       <c r="C9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="E9" s="7" t="s">
         <v>56</v>
       </c>
@@ -1148,7 +1155,9 @@
       <c r="C10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="E10" s="7" t="s">
         <v>49</v>
       </c>
@@ -1166,7 +1175,9 @@
       <c r="C11" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="E11" s="7" t="s">
         <v>67</v>
       </c>
@@ -1184,7 +1195,9 @@
       <c r="C12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7" t="s">
+        <v>76</v>
+      </c>
       <c r="E12" s="13">
         <v>4.99</v>
       </c>
@@ -1202,7 +1215,9 @@
       <c r="C13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="E13" s="7" t="s">
         <v>48</v>
       </c>
@@ -1220,7 +1235,9 @@
       <c r="C14" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="E14" s="13">
         <v>13.14</v>
       </c>
@@ -1279,13 +1296,13 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="105">
+    <row r="7" spans="1:2" ht="90">
       <c r="A7" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:2" ht="75">
+    <row r="8" spans="1:2" ht="60">
       <c r="A8" s="2" t="s">
         <v>70</v>
       </c>

</xml_diff>